<commit_message>
Generación de estadísticas Introducción en el juego del guardado de estadísticas Modo entrenamiento ia vs ia, introducido
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D950C368-CE20-46FF-A3E8-FFF7313647EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F467A2F2-9304-41B3-8391-9494882B542D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Fecha</t>
   </si>
@@ -40,6 +40,21 @@
   </si>
   <si>
     <t>Estructura y lectura/escritura XML</t>
+  </si>
+  <si>
+    <t>Generación de gráficas</t>
+  </si>
+  <si>
+    <t>Modo entrenamiento</t>
+  </si>
+  <si>
+    <t>Entrenamiento IA vs IA básico</t>
+  </si>
+  <si>
+    <t>3 h.</t>
+  </si>
+  <si>
+    <t>1.5 h.</t>
   </si>
 </sst>
 </file>
@@ -418,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y34" sqref="Y34"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,30 +444,54 @@
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4">
         <v>43985</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="4">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creación estructuras base Deep Q-Learning
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F467A2F2-9304-41B3-8391-9494882B542D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB774CF4-E0FF-4564-850C-F2730159A7A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Fecha</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>1.5 h.</t>
+  </si>
+  <si>
+    <t>Investigación</t>
+  </si>
+  <si>
+    <t>Aprendizaje por refuerzo (Deep Q-Learning)</t>
+  </si>
+  <si>
+    <t>Implementación Deep Q-Learning</t>
+  </si>
+  <si>
+    <t>Estructuras básicas (estados y agente)</t>
+  </si>
+  <si>
+    <t>2 h.</t>
   </si>
 </sst>
 </file>
@@ -140,7 +155,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -151,6 +166,9 @@
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16"/>
@@ -433,23 +451,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -459,13 +477,25 @@
       <c r="C2" s="4">
         <v>43986</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="4">
+        <v>43989</v>
+      </c>
+      <c r="E2" s="4">
+        <v>43990</v>
+      </c>
+      <c r="F2" s="4">
+        <v>43991</v>
+      </c>
+      <c r="G2" s="4">
+        <v>43992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -473,7 +503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -481,17 +511,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ampliación Q-Learning Introducido agent controller
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB774CF4-E0FF-4564-850C-F2730159A7A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37E7DE3-0CE9-4001-B0D2-B6FC042217B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Fecha</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>2 h.</t>
+  </si>
+  <si>
+    <t>3.5 h.</t>
+  </si>
+  <si>
+    <t>Algoritmo Q-learning</t>
+  </si>
+  <si>
+    <t>4.5 h.</t>
+  </si>
+  <si>
+    <t>Total horas: 29.5</t>
   </si>
 </sst>
 </file>
@@ -451,23 +463,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -489,13 +502,19 @@
       <c r="G2" s="4">
         <v>43992</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="4">
+        <v>43993</v>
+      </c>
+      <c r="I2" s="4">
+        <v>43996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -503,7 +522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -511,12 +530,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -524,12 +543,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -543,17 +562,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solucionada reescritura de trainingRegister Revisar que al ganar y perder da demasiadas recompensas, hay 13 cuando deberia haber 4 Repensar la asignación de recompensas Revisar también el hacer ataques en el aire
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37E7DE3-0CE9-4001-B0D2-B6FC042217B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD120E0-ECD9-4133-AD85-D6EEA8827546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Fecha</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Total horas: 29.5</t>
+  </si>
+  <si>
+    <t>2.5 h.</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -181,6 +184,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16"/>
@@ -463,16 +467,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -480,7 +486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -508,13 +514,19 @@
       <c r="I2" s="4">
         <v>43996</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="4">
+        <v>43999</v>
+      </c>
+      <c r="K2" s="4">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -522,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -530,12 +542,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -543,12 +555,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -562,20 +574,22 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -584,6 +598,12 @@
       </c>
       <c r="I12" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mirar por que no funciona el multijugador
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB774CF4-E0FF-4564-850C-F2730159A7A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AF96A1-4A91-4B6C-812D-24F65203458E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Fecha</t>
   </si>
@@ -60,16 +60,52 @@
     <t>Investigación</t>
   </si>
   <si>
-    <t>Aprendizaje por refuerzo (Deep Q-Learning)</t>
-  </si>
-  <si>
-    <t>Implementación Deep Q-Learning</t>
-  </si>
-  <si>
     <t>Estructuras básicas (estados y agente)</t>
   </si>
   <si>
     <t>2 h.</t>
+  </si>
+  <si>
+    <t>3.5 h.</t>
+  </si>
+  <si>
+    <t>Algoritmo Q-learning</t>
+  </si>
+  <si>
+    <t>4.5 h.</t>
+  </si>
+  <si>
+    <t>2.5 h.</t>
+  </si>
+  <si>
+    <t>Aprendizaje por refuerzo (Q-Learning)</t>
+  </si>
+  <si>
+    <t>Implementación Q-Learning</t>
+  </si>
+  <si>
+    <t>Aprendizaje por refuerzo (Actor-Critic)</t>
+  </si>
+  <si>
+    <t>1 h.</t>
+  </si>
+  <si>
+    <t>5 h.</t>
+  </si>
+  <si>
+    <t>Servidor</t>
+  </si>
+  <si>
+    <t>Total horas: 75.5</t>
+  </si>
+  <si>
+    <t>Estructuras básicas (conexiones)</t>
+  </si>
+  <si>
+    <t>Servicios en línea</t>
+  </si>
+  <si>
+    <t>Implementación partida en red</t>
   </si>
 </sst>
 </file>
@@ -155,7 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -169,6 +205,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16"/>
@@ -451,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,12 +499,15 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -489,13 +529,61 @@
       <c r="G2" s="4">
         <v>43992</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="4">
+        <v>43993</v>
+      </c>
+      <c r="I2" s="4">
+        <v>43996</v>
+      </c>
+      <c r="J2" s="4">
+        <v>43999</v>
+      </c>
+      <c r="K2" s="4">
+        <v>44000</v>
+      </c>
+      <c r="L2" s="4">
+        <v>44001</v>
+      </c>
+      <c r="M2" s="4">
+        <v>44002</v>
+      </c>
+      <c r="N2" s="4">
+        <v>44003</v>
+      </c>
+      <c r="O2" s="4">
+        <v>44005</v>
+      </c>
+      <c r="P2" s="4">
+        <v>44006</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>44007</v>
+      </c>
+      <c r="R2" s="4">
+        <v>44008</v>
+      </c>
+      <c r="S2" s="4">
+        <v>44010</v>
+      </c>
+      <c r="T2" s="4">
+        <v>44011</v>
+      </c>
+      <c r="U2" s="4">
+        <v>44012</v>
+      </c>
+      <c r="V2" s="4">
+        <v>44013</v>
+      </c>
+      <c r="W2" s="4">
+        <v>44014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -503,7 +591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -511,12 +599,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -524,14 +612,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
@@ -543,17 +631,106 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="N10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
+      <c r="I13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya funnciona en red
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AF96A1-4A91-4B6C-812D-24F65203458E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4BC149-6D17-462A-BCEC-8D060A257691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Fecha</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Implementación partida en red</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +502,7 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -507,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -577,13 +580,16 @@
       <c r="W2" s="4">
         <v>44014</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="4">
+        <v>44015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -591,7 +597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -599,12 +605,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -612,12 +618,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -631,7 +637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -645,12 +651,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -661,7 +667,7 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -681,12 +687,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -708,7 +714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -719,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -731,6 +737,14 @@
       </c>
       <c r="W17" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hecha la base de datos y capa DAO
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4BC149-6D17-462A-BCEC-8D060A257691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABCA4F6-3A0D-4961-A0CB-C7DA742285CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Servidor</t>
   </si>
   <si>
-    <t>Total horas: 75.5</t>
-  </si>
-  <si>
     <t>Estructuras básicas (conexiones)</t>
   </si>
   <si>
@@ -108,7 +105,19 @@
     <t>Implementación partida en red</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8</t>
+    <t>Base de datos</t>
+  </si>
+  <si>
+    <t>Total horas: 97</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5</t>
+  </si>
+  <si>
+    <t>Diseño de la base de datos</t>
+  </si>
+  <si>
+    <t>Implementación con JPA e Hibernate</t>
   </si>
 </sst>
 </file>
@@ -491,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F19" sqref="F19:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,15 +511,15 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -583,13 +592,22 @@
       <c r="X2" s="4">
         <v>44015</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Y2" s="4">
+        <v>44016</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>44018</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>44019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -597,7 +615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -605,12 +623,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -618,12 +636,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -637,7 +655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -651,12 +669,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -667,7 +685,7 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -687,14 +705,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>8</v>
@@ -714,9 +732,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>21</v>
@@ -725,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -741,10 +759,40 @@
       <c r="X17" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplificado el número de estados Solucionado bug ia stats
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABCA4F6-3A0D-4961-A0CB-C7DA742285CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7023990-2330-4DAE-A10A-E97F7D410249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -108,16 +114,16 @@
     <t>Base de datos</t>
   </si>
   <si>
-    <t>Total horas: 97</t>
-  </si>
-  <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5</t>
-  </si>
-  <si>
     <t>Diseño de la base de datos</t>
   </si>
   <si>
     <t>Implementación con JPA e Hibernate</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4</t>
+  </si>
+  <si>
+    <t>Total horas: 106</t>
   </si>
 </sst>
 </file>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:F20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,15 +517,15 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -601,21 +607,33 @@
       <c r="AA2" s="4">
         <v>44019</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AB2" s="4">
+        <v>44020</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>44021</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>44023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AD4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -623,12 +641,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -636,12 +654,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -655,7 +673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -669,12 +687,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -685,7 +703,7 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -704,13 +722,19 @@
       <c r="L13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -732,7 +756,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -743,7 +767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -765,23 +789,26 @@
       <c r="Z17" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Z19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z20" s="1" t="s">
         <v>12</v>
@@ -789,10 +816,13 @@
       <c r="AA20" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizado las stadisticas Metidas las funciones de agregar amigos
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981FB24C-5969-4C3A-A8C3-CC34DC2BCEF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B618AFCF-738C-4938-A23B-02407BEDEFF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>Fecha</t>
   </si>
@@ -120,10 +120,13 @@
     <t>Implementación con JPA e Hibernate</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5</t>
-  </si>
-  <si>
-    <t>Total horas: 112.5</t>
+    <t>Regresión logística</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5</t>
+  </si>
+  <si>
+    <t>Total horas: 124.5</t>
   </si>
 </sst>
 </file>
@@ -209,7 +212,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -224,6 +227,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16"/>
@@ -506,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF24"/>
+  <dimension ref="A1:AH24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN6" sqref="AN6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,15 +523,15 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -622,13 +628,19 @@
       <c r="AF2" s="4">
         <v>44025</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AG2" s="4">
+        <v>44026</v>
+      </c>
+      <c r="AH2" s="4">
+        <v>44026</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -639,20 +651,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -660,12 +675,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -679,7 +694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -693,148 +708,163 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="AH13" s="8"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AC13" s="1" t="s">
+      <c r="AC14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AD13" s="1" t="s">
+      <c r="AD14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AE13" s="1" t="s">
+      <c r="AE14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AF13" s="1" t="s">
+      <c r="AF14" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="AG14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1" t="s">
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="U16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="V18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="W18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y17" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z17" s="1" t="s">
+      <c r="Z18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AC17" s="1" t="s">
+      <c r="AC18" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="AH18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="Z19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="Z20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AA20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AB21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementada la regresión logística Buscar un modo de que de un resultado decente
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B618AFCF-738C-4938-A23B-02407BEDEFF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB0AF55-2E96-4803-A958-878A3DC2A04D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>Fecha</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Investigación</t>
   </si>
   <si>
-    <t>Estructuras básicas (estados y agente)</t>
-  </si>
-  <si>
     <t>2 h.</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Aprendizaje por refuerzo (Q-Learning)</t>
   </si>
   <si>
-    <t>Implementación Q-Learning</t>
-  </si>
-  <si>
     <t>Aprendizaje por refuerzo (Actor-Critic)</t>
   </si>
   <si>
@@ -120,13 +114,22 @@
     <t>Implementación con JPA e Hibernate</t>
   </si>
   <si>
-    <t>Regresión logística</t>
-  </si>
-  <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5</t>
-  </si>
-  <si>
-    <t>Total horas: 124.5</t>
+    <t>Implementación aprendizaje automático</t>
+  </si>
+  <si>
+    <t>Estructuras básicas Q-learning</t>
+  </si>
+  <si>
+    <t>Regresión lineal</t>
+  </si>
+  <si>
+    <t>6 h.</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6</t>
+  </si>
+  <si>
+    <t>Total horas: 130.5</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH24"/>
+  <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,15 +526,15 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -632,15 +635,18 @@
         <v>44026</v>
       </c>
       <c r="AH2" s="4">
-        <v>44026</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>44035</v>
+      </c>
+      <c r="AI2" s="4">
+        <v>44036</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -651,7 +657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -659,15 +665,15 @@
         <v>8</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -675,14 +681,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
@@ -694,177 +700,185 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="AH13" s="8"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="AC14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AD14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AE14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="O17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W18" s="1" t="s">
+      <c r="W19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="X19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC18" s="1" t="s">
+      <c r="Y19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AH18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>26</v>
+      <c r="AH19" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>12</v>
+      <c r="A20" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejoradas las gráficas Mirar por que no funciona el jar
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200CCAF7-B5CB-4FEA-BB2B-EB6F7D168327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2805E330-D9A0-42E1-BC78-5F28FDC63237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
   <si>
     <t>Fecha</t>
   </si>
@@ -129,10 +129,16 @@
     <t>6.5 h.</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5</t>
-  </si>
-  <si>
-    <t>Total horas: 137</t>
+    <t>Unión Q-Learning y regrésión lineal</t>
+  </si>
+  <si>
+    <t>1.5 h</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5</t>
+  </si>
+  <si>
+    <t>Total horas: 146.5</t>
   </si>
 </sst>
 </file>
@@ -518,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ25"/>
+  <dimension ref="A1:AL25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,15 +535,15 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -646,13 +652,19 @@
       <c r="AJ2" s="4">
         <v>44037</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AK2" s="4">
+        <v>44038</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>44039</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -663,7 +675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -673,13 +685,16 @@
       <c r="AH5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AL5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -687,12 +702,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -706,7 +721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -720,7 +735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -728,12 +743,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -745,7 +760,7 @@
       <c r="L13" s="7"/>
       <c r="AH13" s="8"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -780,7 +795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -790,104 +805,118 @@
       <c r="AJ15" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="AK15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U19" s="1" t="s">
+      <c r="U20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="V20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W19" s="1" t="s">
+      <c r="W20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X19" s="1" t="s">
+      <c r="X20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y19" s="1" t="s">
+      <c r="Y20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z19" s="1" t="s">
+      <c r="Z20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC19" s="1" t="s">
+      <c r="AC20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AH19" s="1" t="s">
+      <c r="AH20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z21" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Z22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AA22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AB23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejorada la conexión con el servidor mediante el envio de packets Mirar problema con sendableObject a la hora de enviar
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2805E330-D9A0-42E1-BC78-5F28FDC63237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D0E590-B42F-4002-9F17-CBD17DC257DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Fecha</t>
   </si>
@@ -135,10 +135,10 @@
     <t>1.5 h</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5</t>
-  </si>
-  <si>
-    <t>Total horas: 146.5</t>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5</t>
+  </si>
+  <si>
+    <t>Total horas: 151.5</t>
   </si>
 </sst>
 </file>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL25"/>
+  <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -658,13 +658,16 @@
       <c r="AL2" s="4">
         <v>44039</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AM2" s="4">
+        <v>44040</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -675,7 +678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -689,12 +692,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -702,12 +705,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -721,7 +724,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -735,7 +738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -743,12 +746,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -760,7 +763,7 @@
       <c r="L13" s="7"/>
       <c r="AH13" s="8"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -795,7 +798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -811,8 +814,11 @@
       <c r="AL15" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -820,12 +826,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -846,8 +852,11 @@
       <c r="U18" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AM18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -857,8 +866,11 @@
       <c r="R19" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AM19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -887,12 +899,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -900,7 +912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -914,7 +926,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Mejorada la conexion, y añadidas funcionalidades al servidor
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D0E590-B42F-4002-9F17-CBD17DC257DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7E15EF-AF85-4F19-8B13-4D3F971FDE28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>Fecha</t>
   </si>
@@ -135,10 +135,10 @@
     <t>1.5 h</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5</t>
-  </si>
-  <si>
-    <t>Total horas: 151.5</t>
+    <t>Total horas: 157.5</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6</t>
   </si>
 </sst>
 </file>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM25"/>
+  <dimension ref="A1:AN25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,15 +535,15 @@
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -661,13 +661,16 @@
       <c r="AM2" s="4">
         <v>44040</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AN2" s="4">
+        <v>44041</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -678,7 +681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -692,12 +695,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -705,12 +708,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -724,7 +727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -738,7 +741,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -746,12 +749,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -763,7 +766,7 @@
       <c r="L13" s="7"/>
       <c r="AH13" s="8"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -798,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -818,7 +821,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -826,12 +829,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -855,8 +858,11 @@
       <c r="AM18" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -870,7 +876,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -898,13 +904,16 @@
       <c r="AH20" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -912,7 +921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -926,9 +935,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadidas algunas funciones al servidor Comenzada GUI
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7E15EF-AF85-4F19-8B13-4D3F971FDE28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9881DF71-DB70-44C5-8879-7D456318BAD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
   <si>
     <t>Fecha</t>
   </si>
@@ -135,10 +135,22 @@
     <t>1.5 h</t>
   </si>
   <si>
-    <t>Total horas: 157.5</t>
-  </si>
-  <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6</t>
+    <t>Interfaz de usuario</t>
+  </si>
+  <si>
+    <t>Investigación de Swing</t>
+  </si>
+  <si>
+    <t>Implementación (login y registro)</t>
+  </si>
+  <si>
+    <t>2.5.</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6</t>
+  </si>
+  <si>
+    <t>Total horas: 163.5</t>
   </si>
 </sst>
 </file>
@@ -224,7 +236,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -240,6 +252,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -524,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN25"/>
+  <dimension ref="A1:AO27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +552,7 @@
   <sheetData>
     <row r="1" spans="1:40" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -829,12 +844,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -862,7 +877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -876,7 +891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -907,21 +922,26 @@
       <c r="AN20" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO21" s="9"/>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="Z22" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO22" s="9"/>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -934,10 +954,33 @@
       <c r="AB23" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="AO23" s="9"/>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO24" s="9"/>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="AO25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO26" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Metido registro y login buenos
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9881DF71-DB70-44C5-8879-7D456318BAD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0793859-010A-4010-996B-76128CEFC1FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
   <si>
     <t>Fecha</t>
   </si>
@@ -147,10 +147,13 @@
     <t>2.5.</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6</t>
-  </si>
-  <si>
-    <t>Total horas: 163.5</t>
+    <t>6.5 h</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5</t>
+  </si>
+  <si>
+    <t>Total horas: 170</t>
   </si>
 </sst>
 </file>
@@ -539,26 +542,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO27"/>
+  <dimension ref="A1:AP36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -679,13 +680,19 @@
       <c r="AN2" s="4">
         <v>44041</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AO2" s="4">
+        <v>44042</v>
+      </c>
+      <c r="AP2" s="4">
+        <v>44043</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -696,7 +703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -710,12 +717,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -723,12 +730,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -742,7 +749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -756,7 +763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -764,12 +771,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -781,7 +788,7 @@
       <c r="L13" s="7"/>
       <c r="AH13" s="8"/>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -816,7 +823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -836,7 +843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -844,12 +851,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -877,7 +884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -891,7 +898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -926,13 +933,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO21" s="9"/>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -941,7 +948,7 @@
       </c>
       <c r="AO22" s="9"/>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -956,13 +963,13 @@
       </c>
       <c r="AO23" s="9"/>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO24" s="9"/>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -970,17 +977,20 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="AO26" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="AP26" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refinada creación de botones, texfields y casteos Comenzada lista de amigos
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0793859-010A-4010-996B-76128CEFC1FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3E9832-DFD9-4CC4-A9C1-0C2976F2F41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
   <si>
     <t>Fecha</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Total horas: 170</t>
+  </si>
+  <si>
+    <t>3.5 h</t>
   </si>
 </sst>
 </file>
@@ -542,16 +545,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP36"/>
+  <dimension ref="A1:CJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="CL31" sqref="CL31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -559,7 +564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:42" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:88" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -686,13 +691,151 @@
       <c r="AP2" s="4">
         <v>44043</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AQ2" s="4">
+        <v>44044</v>
+      </c>
+      <c r="AR2" s="4">
+        <v>44045</v>
+      </c>
+      <c r="AS2" s="4">
+        <v>44046</v>
+      </c>
+      <c r="AT2" s="4">
+        <v>44047</v>
+      </c>
+      <c r="AU2" s="4">
+        <v>44048</v>
+      </c>
+      <c r="AV2" s="4">
+        <v>44049</v>
+      </c>
+      <c r="AW2" s="4">
+        <v>44050</v>
+      </c>
+      <c r="AX2" s="4">
+        <v>44051</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>44052</v>
+      </c>
+      <c r="AZ2" s="4">
+        <v>44053</v>
+      </c>
+      <c r="BA2" s="4">
+        <v>44054</v>
+      </c>
+      <c r="BB2" s="4">
+        <v>44055</v>
+      </c>
+      <c r="BC2" s="4">
+        <v>44056</v>
+      </c>
+      <c r="BD2" s="4">
+        <v>44057</v>
+      </c>
+      <c r="BE2" s="4">
+        <v>44058</v>
+      </c>
+      <c r="BF2" s="4">
+        <v>44059</v>
+      </c>
+      <c r="BG2" s="4">
+        <v>44060</v>
+      </c>
+      <c r="BH2" s="4">
+        <v>44061</v>
+      </c>
+      <c r="BI2" s="4">
+        <v>44062</v>
+      </c>
+      <c r="BJ2" s="4">
+        <v>44063</v>
+      </c>
+      <c r="BK2" s="4">
+        <v>44064</v>
+      </c>
+      <c r="BL2" s="4">
+        <v>44065</v>
+      </c>
+      <c r="BM2" s="4">
+        <v>44066</v>
+      </c>
+      <c r="BN2" s="4">
+        <v>44067</v>
+      </c>
+      <c r="BO2" s="4">
+        <v>44068</v>
+      </c>
+      <c r="BP2" s="4">
+        <v>44069</v>
+      </c>
+      <c r="BQ2" s="4">
+        <v>44070</v>
+      </c>
+      <c r="BR2" s="4">
+        <v>44071</v>
+      </c>
+      <c r="BS2" s="4">
+        <v>44072</v>
+      </c>
+      <c r="BT2" s="4">
+        <v>44073</v>
+      </c>
+      <c r="BU2" s="4">
+        <v>44074</v>
+      </c>
+      <c r="BV2" s="4">
+        <v>44075</v>
+      </c>
+      <c r="BW2" s="4">
+        <v>44076</v>
+      </c>
+      <c r="BX2" s="4">
+        <v>44077</v>
+      </c>
+      <c r="BY2" s="4">
+        <v>44078</v>
+      </c>
+      <c r="BZ2" s="4">
+        <v>44079</v>
+      </c>
+      <c r="CA2" s="4">
+        <v>44080</v>
+      </c>
+      <c r="CB2" s="4">
+        <v>44081</v>
+      </c>
+      <c r="CC2" s="4">
+        <v>44082</v>
+      </c>
+      <c r="CD2" s="4">
+        <v>44083</v>
+      </c>
+      <c r="CE2" s="4">
+        <v>44084</v>
+      </c>
+      <c r="CF2" s="4">
+        <v>44085</v>
+      </c>
+      <c r="CG2" s="4">
+        <v>44086</v>
+      </c>
+      <c r="CH2" s="4">
+        <v>44087</v>
+      </c>
+      <c r="CI2" s="4">
+        <v>44088</v>
+      </c>
+      <c r="CJ2" s="4">
+        <v>44089</v>
+      </c>
+    </row>
+    <row r="3" spans="1:88" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -703,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -717,12 +860,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -730,12 +873,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -749,7 +892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -763,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -771,12 +914,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -788,7 +931,7 @@
       <c r="L13" s="7"/>
       <c r="AH13" s="8"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -823,7 +966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -843,7 +986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -851,12 +994,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -884,7 +1027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -898,7 +1041,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -933,13 +1076,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO21" s="9"/>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -948,7 +1091,7 @@
       </c>
       <c r="AO22" s="9"/>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -963,13 +1106,13 @@
       </c>
       <c r="AO23" s="9"/>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO24" s="9"/>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -977,7 +1120,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -986,6 +1129,9 @@
       </c>
       <c r="AP26" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="AQ26" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Introducido gui perfil Bug con el pop up de añadir amigo y la tabla del historial
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3E9832-DFD9-4CC4-A9C1-0C2976F2F41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E6D37E-3E1F-4A22-AF02-063357036EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
   <si>
     <t>Fecha</t>
   </si>
@@ -150,13 +150,25 @@
     <t>6.5 h</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5</t>
-  </si>
-  <si>
-    <t>Total horas: 170</t>
-  </si>
-  <si>
     <t>3.5 h</t>
+  </si>
+  <si>
+    <t>5.5 h.</t>
+  </si>
+  <si>
+    <t>Implementación menú principal</t>
+  </si>
+  <si>
+    <t>Implementación perfil</t>
+  </si>
+  <si>
+    <t>7.5 h.</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5</t>
+  </si>
+  <si>
+    <t>Total horas: 191.5</t>
   </si>
 </sst>
 </file>
@@ -548,7 +560,7 @@
   <dimension ref="A1:CJ36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CL31" sqref="CL31"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +570,7 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -994,12 +1006,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1041,7 +1053,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1076,13 +1088,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO21" s="9"/>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1103,7 @@
       </c>
       <c r="AO22" s="9"/>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1106,13 +1118,13 @@
       </c>
       <c r="AO23" s="9"/>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO24" s="9"/>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1120,7 +1132,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1130,13 +1142,32 @@
       <c r="AP26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AQ26" s="1" t="s">
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="AQ27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT28" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introducida selección de personaje y mapa                                         Introducidas algunas peticiones al servidor                                         Mirar problema con peticiones duplicadas
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E6D37E-3E1F-4A22-AF02-063357036EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2121BA5F-11DC-4B92-BCE1-5C3DC80DEAD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>Fecha</t>
   </si>
@@ -165,10 +165,13 @@
     <t>7.5 h.</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5</t>
-  </si>
-  <si>
-    <t>Total horas: 191.5</t>
+    <t>Inclusión de peticiones al servidor</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5</t>
+  </si>
+  <si>
+    <t>Total horas: 200</t>
   </si>
 </sst>
 </file>
@@ -559,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +573,7 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1006,12 +1009,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1088,13 +1091,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO21" s="9"/>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1103,7 +1106,7 @@
       </c>
       <c r="AO22" s="9"/>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1118,13 +1121,13 @@
       </c>
       <c r="AO23" s="9"/>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO24" s="9"/>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
@@ -1157,17 +1160,28 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
       <c r="AT28" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="AU28" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU29" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introducidas algunas peticiones al servidor Solucionado problema con el semaforo de notificaciones Solucionado problema con peticiones duplicadas Mirar problema al cargar partidas de la base de datos
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2121BA5F-11DC-4B92-BCE1-5C3DC80DEAD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C4B28C-2916-4CBC-BED6-98BE4154EAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
   <si>
     <t>Fecha</t>
   </si>
@@ -168,10 +162,13 @@
     <t>Inclusión de peticiones al servidor</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5</t>
-  </si>
-  <si>
-    <t>Total horas: 200</t>
+    <t>7 h.</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7</t>
+  </si>
+  <si>
+    <t>Total horas: 207</t>
   </si>
 </sst>
 </file>
@@ -562,9 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -573,7 +568,7 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1009,12 +1004,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1042,7 +1037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1056,7 +1051,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1091,13 +1086,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO21" s="9"/>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1106,7 +1101,7 @@
       </c>
       <c r="AO22" s="9"/>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1121,13 +1116,13 @@
       </c>
       <c r="AO23" s="9"/>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO24" s="9"/>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1135,7 +1130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1146,7 +1141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
@@ -1160,7 +1155,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
@@ -1171,17 +1166,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AU29" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="AV29" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introducidas notificaciones de amistad y mensajes (de mensajes falta al cerrar char) Mejorados pop ups Sigue estando el problema del multiplayer según la persona
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C4B28C-2916-4CBC-BED6-98BE4154EAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4294AE-A9F1-4C78-9DC3-79CBDF339003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>Fecha</t>
   </si>
@@ -165,10 +165,16 @@
     <t>7 h.</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7</t>
-  </si>
-  <si>
-    <t>Total horas: 207</t>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5</t>
+  </si>
+  <si>
+    <t>Total horas: 220</t>
+  </si>
+  <si>
+    <t>Implementación notificaciones</t>
+  </si>
+  <si>
+    <t>Implementación lista de amigos</t>
   </si>
 </sst>
 </file>
@@ -1004,12 +1010,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1037,7 +1043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1051,7 +1057,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1086,13 +1092,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO21" s="9"/>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1101,7 +1107,7 @@
       </c>
       <c r="AO22" s="9"/>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1116,13 +1122,13 @@
       </c>
       <c r="AO23" s="9"/>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO24" s="9"/>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1141,7 +1147,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
@@ -1155,26 +1161,51 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AT28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AU28" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AU29" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AV29" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AX31" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mejoradas notificaciones mensajes Introducidas verificación de cuenta y recuperación de cuenta, y empezada cambio de contraseña
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4294AE-A9F1-4C78-9DC3-79CBDF339003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CF4215-FC69-42B1-8179-3EDD7BCA46E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Fecha</t>
   </si>
@@ -165,16 +165,19 @@
     <t>7 h.</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5</t>
-  </si>
-  <si>
-    <t>Total horas: 220</t>
-  </si>
-  <si>
     <t>Implementación notificaciones</t>
   </si>
   <si>
     <t>Implementación lista de amigos</t>
+  </si>
+  <si>
+    <t>Implementación verificación y recuperación de cuenta</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7</t>
+  </si>
+  <si>
+    <t>Total horas: 227</t>
   </si>
 </sst>
 </file>
@@ -565,16 +568,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G23" sqref="G22:G23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" customWidth="1"/>
+    <col min="1" max="1" width="55" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1010,12 +1015,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1043,7 +1048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1057,7 +1062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1092,13 +1097,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO21" s="9"/>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1107,7 +1112,7 @@
       </c>
       <c r="AO22" s="9"/>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1122,13 +1127,13 @@
       </c>
       <c r="AO23" s="9"/>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO24" s="9"/>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1136,7 +1141,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1147,7 +1152,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
@@ -1161,15 +1166,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AT28" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>42</v>
       </c>
@@ -1180,9 +1185,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AU30" s="1" t="s">
         <v>11</v>
@@ -1194,23 +1199,34 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY31" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AU31" s="1" t="s">
+      <c r="AU32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AW31" s="1" t="s">
+      <c r="AW32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AX31" s="1" t="s">
+      <c r="AX32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AY32" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incluido cambio de contraseña Conectada selección de personaje y sincronización Mejorada connection con los acks aparte
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CF4215-FC69-42B1-8179-3EDD7BCA46E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BFFEF6-9765-4C90-B7EB-0710539E52CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
   <si>
     <t>Fecha</t>
   </si>
@@ -174,10 +174,19 @@
     <t>Implementación verificación y recuperación de cuenta</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7</t>
-  </si>
-  <si>
-    <t>Total horas: 227</t>
+    <t>Implementación selección personaje y mapa</t>
+  </si>
+  <si>
+    <t>Implementación cambio de contraseña</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5</t>
+  </si>
+  <si>
+    <t>Total horas: 234.5</t>
+  </si>
+  <si>
+    <t>0.5 h.</t>
   </si>
 </sst>
 </file>
@@ -568,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G22:G23"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AZ35" sqref="AZ35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +588,7 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1015,12 +1024,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1048,7 +1057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1062,7 +1071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1097,13 +1106,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO21" s="9"/>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1112,7 +1121,7 @@
       </c>
       <c r="AO22" s="9"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1127,13 +1136,13 @@
       </c>
       <c r="AO23" s="9"/>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO24" s="9"/>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1141,7 +1150,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
@@ -1166,7 +1175,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>47</v>
       </c>
@@ -1174,7 +1183,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>42</v>
       </c>
@@ -1185,7 +1194,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>46</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>48</v>
       </c>
@@ -1207,26 +1216,45 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AU33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ33" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AU32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW32" s="1" t="s">
+      <c r="AW34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AX32" s="1" t="s">
+      <c r="AX34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AY32" s="1" t="s">
+      <c r="AY34" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="AZ34" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introducida pantalla final partida Intentado UPnP Corregido bug al reconectarse cliente tras caida
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BFFEF6-9765-4C90-B7EB-0710539E52CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77167177-144E-4031-8EC2-5B5A53906312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t>Fecha</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Implementación verificación y recuperación de cuenta</t>
   </si>
   <si>
-    <t>Implementación selección personaje y mapa</t>
-  </si>
-  <si>
     <t>Implementación cambio de contraseña</t>
   </si>
   <si>
@@ -187,6 +184,12 @@
   </si>
   <si>
     <t>0.5 h.</t>
+  </si>
+  <si>
+    <t>Implementación selección personaje y mapa, y final partida</t>
+  </si>
+  <si>
+    <t>UPnP (e intento de implementación)</t>
   </si>
 </sst>
 </file>
@@ -575,20 +578,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ36"/>
+  <dimension ref="A1:CJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AZ35" sqref="AZ35"/>
+    <sheetView tabSelected="1" topLeftCell="AA6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BB12" sqref="BB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1"/>
+    <col min="1" max="1" width="60.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -945,316 +948,333 @@
       </c>
     </row>
     <row r="12" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="AH13" s="8"/>
     </row>
     <row r="14" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG14" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="AH14" s="8"/>
     </row>
     <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AL15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC15" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="AI16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="AK16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="AL16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1" t="s">
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="U19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AM18" s="1" t="s">
+      <c r="AM19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AN18" s="1" t="s">
+      <c r="AN19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AM19" s="1" t="s">
+      <c r="AM20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="U21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="V21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W20" s="1" t="s">
+      <c r="W21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X20" s="1" t="s">
+      <c r="X21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y20" s="1" t="s">
+      <c r="Y21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z20" s="1" t="s">
+      <c r="Z21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC20" s="1" t="s">
+      <c r="AC21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AH20" s="1" t="s">
+      <c r="AH21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AN20" s="1" t="s">
+      <c r="AN21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AO20" s="1" t="s">
+      <c r="AO21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AO21" s="9"/>
-    </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="AO22" s="9"/>
+    </row>
+    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="Z22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO22" s="9"/>
-    </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="Z23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AA23" s="1" t="s">
+      <c r="AO23" s="9"/>
+    </row>
+    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AB23" s="1" t="s">
+      <c r="AB24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AO23" s="9"/>
-    </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="AO24" s="9"/>
+    </row>
+    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AO24" s="9"/>
-    </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="AO25" s="9"/>
+    </row>
+    <row r="26" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AO25" s="1" t="s">
+      <c r="AO26" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AO26" s="1" t="s">
+      <c r="AO27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AP26" s="1" t="s">
+      <c r="AP27" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AQ27" s="1" t="s">
+      <c r="AQ28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AR27" s="1" t="s">
+      <c r="AR28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AS27" s="1" t="s">
+      <c r="AS28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AT28" s="1" t="s">
+      <c r="AT29" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="30" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="AU29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV29" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="AU30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AW30" s="1" t="s">
+      <c r="AV30" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AX30" s="1" t="s">
+      <c r="AX31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="BA31" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AY31" s="1" t="s">
+      <c r="AY32" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ32" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AU33" s="1" t="s">
+      <c r="AZ33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AZ33" s="1" t="s">
+      <c r="AZ34" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="BB34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AW34" s="1" t="s">
+      <c r="AW35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AX34" s="1" t="s">
+      <c r="AX35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AY34" s="1" t="s">
+      <c r="AY35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AZ34" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>51</v>
+      <c r="AZ35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introducido SSL entre el servidor y el cliente
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77167177-144E-4031-8EC2-5B5A53906312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1688781C-0A52-4301-846F-7A44EA5689EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="55">
   <si>
     <t>Fecha</t>
   </si>
@@ -159,9 +159,6 @@
     <t>7.5 h.</t>
   </si>
   <si>
-    <t>Inclusión de peticiones al servidor</t>
-  </si>
-  <si>
     <t>7 h.</t>
   </si>
   <si>
@@ -177,12 +174,6 @@
     <t>Implementación cambio de contraseña</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5</t>
-  </si>
-  <si>
-    <t>Total horas: 234.5</t>
-  </si>
-  <si>
     <t>0.5 h.</t>
   </si>
   <si>
@@ -190,6 +181,15 @@
   </si>
   <si>
     <t>UPnP (e intento de implementación)</t>
+  </si>
+  <si>
+    <t>Implementación SSL en comunicación cliente-servidor</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6</t>
+  </si>
+  <si>
+    <t>Total horas: 246.5</t>
   </si>
 </sst>
 </file>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BB12" sqref="BB12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +591,7 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="12" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="BB12" s="1" t="s">
         <v>12</v>
@@ -1027,7 +1027,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1035,12 +1035,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1116,165 +1116,168 @@
       <c r="AO21" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="AW21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AX21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AY21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA21" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AO22" s="9"/>
-    </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="AO23" s="9"/>
+    </row>
+    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="Z23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO23" s="9"/>
-    </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="Z24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AA24" s="1" t="s">
+      <c r="AO24" s="9"/>
+    </row>
+    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AB24" s="1" t="s">
+      <c r="AB25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AO24" s="9"/>
-    </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="AO25" s="9"/>
+    </row>
+    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AO25" s="9"/>
-    </row>
-    <row r="26" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="AO26" s="9"/>
+    </row>
+    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AO26" s="1" t="s">
+      <c r="AO27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AO27" s="1" t="s">
+      <c r="AO28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AP27" s="1" t="s">
+      <c r="AP28" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AQ28" s="1" t="s">
+      <c r="AQ29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AR28" s="1" t="s">
+      <c r="AR29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AS28" s="1" t="s">
+      <c r="AS29" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AT29" s="1" t="s">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="AU30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV30" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="AU31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AW31" s="1" t="s">
+      <c r="AV31" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AX31" s="1" t="s">
+      <c r="AX32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="BA31" s="1" t="s">
+      <c r="BA32" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY32" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ33" s="1" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="AY33" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU34" s="1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="AZ34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB34" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AX35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY35" s="1" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="AU35" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="AZ35" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB35" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comenzada integración de la ia en el servidor
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA020EA-4A1C-4886-B5E5-94AC62A71358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0A77AE-AB71-4AFA-A202-4FBDFFA052F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="59">
   <si>
     <t>Fecha</t>
   </si>
@@ -186,12 +186,6 @@
     <t>Implementación SSL en comunicación cliente-servidor</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5</t>
-  </si>
-  <si>
-    <t>Total horas: 257</t>
-  </si>
-  <si>
     <t>Depuración y corrección de problemas</t>
   </si>
   <si>
@@ -199,6 +193,15 @@
   </si>
   <si>
     <t>4.5 h</t>
+  </si>
+  <si>
+    <t>Integración IA en el servidor</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7</t>
+  </si>
+  <si>
+    <t>Total horas: 264</t>
   </si>
 </sst>
 </file>
@@ -589,9 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BE37" sqref="BE37"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -600,7 +601,7 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1036,7 +1037,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1044,12 +1045,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1094,7 +1095,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>52</v>
       </c>
@@ -1155,157 +1156,165 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AO23" s="9"/>
-    </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="AO24" s="9"/>
+    </row>
+    <row r="25" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="Z24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO24" s="9"/>
-    </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="Z25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AA25" s="1" t="s">
+      <c r="AO25" s="9"/>
+    </row>
+    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AB25" s="1" t="s">
+      <c r="AB26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AO25" s="9"/>
-    </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="AO26" s="9"/>
+    </row>
+    <row r="27" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AO26" s="9"/>
-    </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="AO27" s="9"/>
+    </row>
+    <row r="28" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AO27" s="1" t="s">
+      <c r="AO28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AO28" s="1" t="s">
+      <c r="AO29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AP28" s="1" t="s">
+      <c r="AP29" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AQ29" s="1" t="s">
+      <c r="AQ30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AR29" s="1" t="s">
+      <c r="AR30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AS29" s="1" t="s">
+      <c r="AS30" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AT30" s="1" t="s">
+      <c r="AT31" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="AU31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV31" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="AU32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AW32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AX32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="BA32" s="1" t="s">
-        <v>2</v>
+      <c r="AV32" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AY33" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
+      </c>
+      <c r="AU33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BA33" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AZ34" s="1" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="AY34" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ35" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AU35" s="1" t="s">
+      <c r="AU36" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AZ35" s="1" t="s">
+      <c r="AZ36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="BB35" s="1" t="s">
+      <c r="BB36" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE38" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE37" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terminada integración de la IA Mejoradas cosas de la comunicación servidor-cliente
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0A77AE-AB71-4AFA-A202-4FBDFFA052F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC8C93F-D749-42A2-A7FE-BE8AAAC964F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="59">
   <si>
     <t>Fecha</t>
   </si>
@@ -189,19 +189,19 @@
     <t>Depuración y corrección de problemas</t>
   </si>
   <si>
-    <t>Pruebas y corrección de bugs en la gui</t>
-  </si>
-  <si>
     <t>4.5 h</t>
   </si>
   <si>
     <t>Integración IA en el servidor</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7</t>
-  </si>
-  <si>
-    <t>Total horas: 264</t>
+    <t>Pruebas y corrección de bugs</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6</t>
+  </si>
+  <si>
+    <t>Total horas: 270</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1037,7 +1039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1045,12 +1047,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1078,7 +1080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1095,7 +1097,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1145,7 +1147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>52</v>
       </c>
@@ -1156,21 +1158,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="BG23" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO24" s="9"/>
     </row>
-    <row r="25" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
@@ -1179,7 +1184,7 @@
       </c>
       <c r="AO25" s="9"/>
     </row>
-    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
@@ -1194,13 +1199,13 @@
       </c>
       <c r="AO26" s="9"/>
     </row>
-    <row r="27" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO27" s="9"/>
     </row>
-    <row r="28" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1208,7 +1213,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -1219,7 +1224,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>41</v>
       </c>
@@ -1233,7 +1238,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>46</v>
       </c>
@@ -1241,7 +1246,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
@@ -1252,7 +1257,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>45</v>
       </c>
@@ -1269,7 +1274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>47</v>
       </c>
@@ -1277,7 +1282,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>48</v>
       </c>
@@ -1285,7 +1290,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>50</v>
       </c>
@@ -1299,20 +1304,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE38" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BE38" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BH38" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Mejorado modo entrenamiento Nota para conexión de partida: 1-Establecer conexión udp con el servidor, haciendo que el cliente genere el puerto libremente 2-Una vez ambas conexiones se hayan generado correctamente, enviar la respuesta de partida con el puerto tb
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BCA770-0AC6-491C-A1C1-C00EA0723D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208C11B9-057E-4BA1-91FE-0F706844A1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="61">
   <si>
     <t>Fecha</t>
   </si>
@@ -201,10 +201,13 @@
     <t>Normativa acerca del TFG y la memoria</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5</t>
-  </si>
-  <si>
-    <t>Total horas: 292</t>
+    <t>Documentación y memoria</t>
+  </si>
+  <si>
+    <t>Total horas: 301.5</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1031,7 +1036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -1051,7 +1056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1059,12 +1064,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1091,8 +1096,11 @@
       <c r="AN20" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BO20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -1112,7 +1120,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1162,7 +1170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
@@ -1173,7 +1181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>55</v>
       </c>
@@ -1184,13 +1192,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO25" s="9"/>
     </row>
-    <row r="26" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1199,7 +1207,7 @@
       </c>
       <c r="AO26" s="9"/>
     </row>
-    <row r="27" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1214,13 +1222,13 @@
       </c>
       <c r="AO27" s="9"/>
     </row>
-    <row r="28" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO28" s="9"/>
     </row>
-    <row r="29" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -1228,7 +1236,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
@@ -1239,7 +1247,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -1253,7 +1261,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>46</v>
       </c>
@@ -1261,7 +1269,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -1272,7 +1280,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -1289,7 +1297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -1297,7 +1305,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -1305,7 +1313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
@@ -1319,12 +1327,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -1341,9 +1349,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="BN40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solucionado problema de que solo algunos podian jugar en red Comenzado despliegue en google cloud
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208C11B9-057E-4BA1-91FE-0F706844A1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F325B54-71F2-483F-8BDC-8FE997B0D931}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
   <si>
     <t>Fecha</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7</t>
+  </si>
+  <si>
+    <t>Despliegue del servidor en google cloud</t>
   </si>
 </sst>
 </file>
@@ -598,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BP41" sqref="BP41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1064,12 +1067,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1099,8 +1102,11 @@
       <c r="BO20" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BP20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -1120,7 +1126,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
@@ -1181,7 +1187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>55</v>
       </c>
@@ -1192,13 +1198,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AO25" s="9"/>
     </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1207,7 +1213,7 @@
       </c>
       <c r="AO26" s="9"/>
     </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1222,13 +1228,13 @@
       </c>
       <c r="AO27" s="9"/>
     </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO28" s="9"/>
     </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -1236,7 +1242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
@@ -1247,7 +1253,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>46</v>
       </c>
@@ -1269,7 +1275,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -1280,7 +1286,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -1297,7 +1303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -1305,7 +1311,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -1313,7 +1319,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
@@ -1327,12 +1333,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -1349,7 +1355,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>58</v>
       </c>
@@ -1360,7 +1366,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="BP41" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Actualizado Cronograma.xlsx Corregido error al escribir el xml de las dos ias
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAFB514-D24C-489F-8A49-597D0C118AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506DB346-DE8B-4700-B1A3-C34D00061FE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="63">
   <si>
     <t>Fecha</t>
   </si>
@@ -210,10 +210,10 @@
     <t xml:space="preserve"> 2 h.</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7+6+6+3.5+5.5</t>
-  </si>
-  <si>
-    <t>Total horas: 322.5</t>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7+6+6+3.5+5.5+5.5+4+6</t>
+  </si>
+  <si>
+    <t>Total horas: 338</t>
   </si>
 </sst>
 </file>
@@ -604,9 +604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1281,7 +1279,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -1292,7 +1290,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -1309,7 +1307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -1317,7 +1315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -1325,7 +1323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
@@ -1339,12 +1337,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -1364,7 +1362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>58</v>
       </c>
@@ -1380,8 +1378,17 @@
       <c r="BS40" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BU40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BV40" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>59</v>
       </c>
@@ -1392,7 +1399,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Corregida k-fold cross validation
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506DB346-DE8B-4700-B1A3-C34D00061FE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75DF6A4-002B-4A9D-9B18-949CA69C3138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
   <si>
     <t>Fecha</t>
   </si>
@@ -210,10 +210,10 @@
     <t xml:space="preserve"> 2 h.</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7+6+6+3.5+5.5+5.5+4+6</t>
-  </si>
-  <si>
-    <t>Total horas: 338</t>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7+6+6+3.5+5.5+5.5+4+6+6</t>
+  </si>
+  <si>
+    <t>Total horas: 344</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1279,7 +1281,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -1290,7 +1292,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -1307,7 +1309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -1315,7 +1317,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -1323,7 +1325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
@@ -1337,12 +1339,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -1362,7 +1364,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>58</v>
       </c>
@@ -1387,8 +1389,11 @@
       <c r="BV40" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="BW40" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>59</v>
       </c>
@@ -1399,7 +1404,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Corregido bug de cuentas simultaneas y de final de partida
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75DF6A4-002B-4A9D-9B18-949CA69C3138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3826930B-0FA3-4D61-A3E4-F113E00F2333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="63">
   <si>
     <t>Fecha</t>
   </si>
@@ -210,10 +210,10 @@
     <t xml:space="preserve"> 2 h.</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7+6+6+3.5+5.5+5.5+4+6+6</t>
-  </si>
-  <si>
-    <t>Total horas: 344</t>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7+6+6+3.5+5.5+5.5+4+6+6+6.5+5</t>
+  </si>
+  <si>
+    <t>Total horas: 355.5</t>
   </si>
 </sst>
 </file>
@@ -602,18 +602,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ43"/>
+  <dimension ref="A1:CR43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:96" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -621,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:88" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:96" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -886,13 +884,37 @@
       <c r="CJ2" s="4">
         <v>44089</v>
       </c>
-    </row>
-    <row r="3" spans="1:88" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="CK2" s="4">
+        <v>44090</v>
+      </c>
+      <c r="CL2" s="4">
+        <v>44091</v>
+      </c>
+      <c r="CM2" s="4">
+        <v>44092</v>
+      </c>
+      <c r="CN2" s="4">
+        <v>44093</v>
+      </c>
+      <c r="CO2" s="4">
+        <v>44094</v>
+      </c>
+      <c r="CP2" s="4">
+        <v>44095</v>
+      </c>
+      <c r="CQ2" s="4">
+        <v>44096</v>
+      </c>
+      <c r="CR2" s="4">
+        <v>44097</v>
+      </c>
+    </row>
+    <row r="3" spans="1:96" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -903,7 +925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -917,12 +939,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -933,12 +955,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -952,7 +974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -966,7 +988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -974,7 +996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
@@ -982,7 +1004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
@@ -990,12 +1012,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1007,7 +1029,7 @@
       <c r="L15" s="7"/>
       <c r="AH15" s="8"/>
     </row>
-    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1281,7 +1303,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -1292,7 +1314,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -1309,7 +1331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -1317,7 +1339,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -1325,7 +1347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
@@ -1339,12 +1361,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -1364,7 +1386,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>58</v>
       </c>
@@ -1392,8 +1414,14 @@
       <c r="BW40" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="BX40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="BY40" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>59</v>
       </c>
@@ -1404,7 +1432,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Corregidos algunos detalles de la interfaz
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueSac\Desktop\Tools\IntellJIdeaWorkspace\TFG\TFG-Fatal-Fury-2-Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A828ABD-F002-4833-8A7D-D535B618D643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784BC5A1-9DA2-444B-BC9F-F3DAB865B97F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="64">
   <si>
     <t>Fecha</t>
   </si>
@@ -210,10 +210,13 @@
     <t xml:space="preserve"> 2 h.</t>
   </si>
   <si>
-    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7+6+6+3.5+5.5+5.5+4+6+6+6.5+5+3+5+6</t>
-  </si>
-  <si>
-    <t>Total horas: 369.5</t>
+    <t>5.5 h</t>
+  </si>
+  <si>
+    <t>4+3+1.5+4+4+3+2+3.5+4.5+4.5+5+1+5+3+4+5+4+4+3+4+3.5+8+3.5+5+5+5+4+3+3.5+4+2.5+5.5+6+6.5+5+4.5+5+6+6+6.5+3.5+5.5+6+7.5+8.5+7+5.5+7.5+7+6.5+6+6+6+4.5+7+6+7+5.5+6+3.5+2.5+7+6+6+3.5+5.5+5.5+4+6+6+6.5+5+3+5+6+5.5+6.5+5</t>
+  </si>
+  <si>
+    <t>Total horas: 386.5</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -613,7 +618,7 @@
   <sheetData>
     <row r="1" spans="1:96" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1303,7 +1308,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -1314,7 +1319,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -1331,7 +1336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -1339,7 +1344,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -1347,7 +1352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
@@ -1361,12 +1366,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -1386,7 +1391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>58</v>
       </c>
@@ -1429,8 +1434,17 @@
       <c r="CC40" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="CD40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="CE40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="CF40" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>59</v>
       </c>
@@ -1441,9 +1455,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>